<commit_message>
updates to the predictor outputs
I turned the output up from 6 to 8 predictions and then resized the plots and colored the spreadsheet.
</commit_message>
<xml_diff>
--- a/data/IN/outputs/587734/t_set_test.xlsx
+++ b/data/IN/outputs/587734/t_set_test.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="218">
   <si>
     <t>Row</t>
   </si>
@@ -671,7 +671,13 @@
     <t>t8</t>
   </si>
   <si>
-    <t>t8_check</t>
+    <t>t9</t>
+  </si>
+  <si>
+    <t>t10</t>
+  </si>
+  <si>
+    <t>t10_check</t>
   </si>
 </sst>
 </file>
@@ -1023,15 +1029,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O102"/>
+  <dimension ref="A1:Q102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:O102"/>
+      <selection activeCell="S14" sqref="S14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1077,8 +1083,14 @@
       <c r="O1" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P1" t="s">
+        <v>216</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -1092,28 +1104,34 @@
         <v>0.93411717916192871</v>
       </c>
       <c r="I2">
-        <v>0.90432736042887785</v>
+        <v>0.97206835256297497</v>
       </c>
       <c r="J2">
-        <v>0.85898587307369689</v>
+        <v>0.95622408159473105</v>
       </c>
       <c r="K2">
-        <v>0.82973479128049743</v>
+        <v>0.92638299865355422</v>
       </c>
       <c r="L2">
-        <v>0.70482870660808428</v>
+        <v>0.98673017229691207</v>
       </c>
       <c r="M2">
-        <v>0.58893714700311484</v>
+        <v>0.94015428045087157</v>
       </c>
       <c r="N2">
-        <v>0.481796154261872</v>
+        <v>0.88706711091009072</v>
       </c>
       <c r="O2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.93456133091970361</v>
+      </c>
+      <c r="P2">
+        <v>0.92248805283569524</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -1127,28 +1145,34 @@
         <v>0.94245376111685564</v>
       </c>
       <c r="I3">
-        <v>0.90900960898373406</v>
+        <v>0.97328432189994185</v>
       </c>
       <c r="J3">
-        <v>0.86636346528754105</v>
+        <v>0.95395054314312377</v>
       </c>
       <c r="K3">
-        <v>0.8325038769086992</v>
+        <v>0.92303754136961325</v>
       </c>
       <c r="L3">
-        <v>0.70099942804376358</v>
+        <v>0.98456899921993157</v>
       </c>
       <c r="M3">
-        <v>0.59834818628217168</v>
+        <v>0.93869959751833942</v>
       </c>
       <c r="N3">
-        <v>0.46949077504611364</v>
+        <v>0.89341190698664452</v>
       </c>
       <c r="O3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.93862512143031029</v>
+      </c>
+      <c r="P3">
+        <v>0.91067872339803313</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -1174,28 +1198,34 @@
         <v>0.25</v>
       </c>
       <c r="I4">
-        <v>0.11051212938005392</v>
+        <v>0.4173553719008265</v>
       </c>
       <c r="J4">
-        <v>4.9769923496033659E-2</v>
+        <v>0.21379523981620119</v>
       </c>
       <c r="K4">
-        <v>2.2856881951298709E-2</v>
+        <v>7.6716310826446449E-2</v>
       </c>
       <c r="L4">
-        <v>7.7368542262487537E-3</v>
+        <v>0.40487005842992674</v>
       </c>
       <c r="M4">
-        <v>2.978804648413018E-3</v>
+        <v>3.9368824580687641E-2</v>
       </c>
       <c r="N4">
-        <v>1.2667583787656404E-3</v>
+        <v>1.2145351112396657E-2</v>
       </c>
       <c r="O4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+        <v>1.2305296431952504E-2</v>
+      </c>
+      <c r="P4">
+        <v>5.5988071757079438E-3</v>
+      </c>
+      <c r="Q4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -1209,28 +1239,34 @@
         <v>0.99999690998855084</v>
       </c>
       <c r="I5">
-        <v>0.99999950645522317</v>
+        <v>0.9999970571315201</v>
       </c>
       <c r="J5">
-        <v>0.99</v>
+        <v>0.99999932422866877</v>
       </c>
       <c r="K5">
-        <v>0.99878123095673366</v>
+        <v>0.99999993856620495</v>
       </c>
       <c r="L5">
-        <v>0.9998746469221641</v>
+        <v>0.99999986508657768</v>
       </c>
       <c r="M5">
-        <v>0.99998443721959973</v>
+        <v>0.99999991626063023</v>
       </c>
       <c r="N5">
-        <v>0.99999726003873901</v>
+        <v>0.9999999875015857</v>
       </c>
       <c r="O5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.99999999418933361</v>
+      </c>
+      <c r="P5">
+        <v>0.99999999877000489</v>
+      </c>
+      <c r="Q5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -1244,28 +1280,34 @@
         <v>0.99997802694524307</v>
       </c>
       <c r="I6">
-        <v>0.99999642292528212</v>
+        <v>0.99996945235654766</v>
       </c>
       <c r="J6">
-        <v>0.99999932929654112</v>
+        <v>0.99999022455103581</v>
       </c>
       <c r="K6">
-        <v>0.99999984267441655</v>
+        <v>0.99999874964121727</v>
       </c>
       <c r="L6">
-        <v>0.99999997987695755</v>
+        <v>0.99999706812916356</v>
       </c>
       <c r="M6">
-        <v>0.99999999688571961</v>
+        <v>0.99999878536571052</v>
       </c>
       <c r="N6">
-        <v>0.9999999992214299</v>
+        <v>0.99999977225584591</v>
       </c>
       <c r="O6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.99999982105815588</v>
+      </c>
+      <c r="P6">
+        <v>0.99999995802598141</v>
+      </c>
+      <c r="Q6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -1279,28 +1321,34 @@
         <v>0.88616663738514578</v>
       </c>
       <c r="I7">
-        <v>0.79719824794032479</v>
+        <v>0.94462975754778922</v>
       </c>
       <c r="J7">
-        <v>0.68681900139515195</v>
+        <v>0.87626228018114938</v>
       </c>
       <c r="K7">
-        <v>0.57503833169762431</v>
+        <v>0.77055217523702868</v>
       </c>
       <c r="L7">
-        <v>0.34689370539175157</v>
+        <v>0.93769513616902234</v>
       </c>
       <c r="M7">
-        <v>0.22342352148938111</v>
+        <v>0.66339576102142317</v>
       </c>
       <c r="N7">
-        <v>0.13683743954573591</v>
+        <v>0.47459821392604329</v>
       </c>
       <c r="O7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.57402467137331437</v>
+      </c>
+      <c r="P7">
+        <v>0.45664278219464421</v>
+      </c>
+      <c r="Q7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -1314,28 +1362,34 @@
         <v>0.98960942196562796</v>
       </c>
       <c r="I8">
-        <v>0.98912001583658471</v>
+        <v>0.99747726133369774</v>
       </c>
       <c r="J8">
-        <v>0.98858886367950016</v>
+        <v>0.99716281368536241</v>
       </c>
       <c r="K8">
-        <v>0.9901854815018476</v>
+        <v>0.99690568576094185</v>
       </c>
       <c r="L8">
-        <v>0.98605823273423965</v>
+        <v>0.99897455979567229</v>
       </c>
       <c r="M8">
-        <v>0.98572708146779675</v>
+        <v>0.99730797067249244</v>
       </c>
       <c r="N8">
-        <v>0.98324009563291193</v>
+        <v>0.99678620278810015</v>
       </c>
       <c r="O8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.99864290116828258</v>
+      </c>
+      <c r="P8">
+        <v>0.99883444162153745</v>
+      </c>
+      <c r="Q8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -1349,28 +1403,34 @@
         <v>0.80183589397647659</v>
       </c>
       <c r="I9">
-        <v>0.66097003450834513</v>
+        <v>0.92622090644116506</v>
       </c>
       <c r="J9">
-        <v>0.54250875445053426</v>
+        <v>0.87501961203074663</v>
       </c>
       <c r="K9">
-        <v>0.43896061315693091</v>
+        <v>0.7636687289958739</v>
       </c>
       <c r="L9">
-        <v>0.25801493617321392</v>
+        <v>0.91483600161246759</v>
       </c>
       <c r="M9">
-        <v>0.16883664376802918</v>
+        <v>0.77932900452314469</v>
       </c>
       <c r="N9">
-        <v>0.1187338842015969</v>
+        <v>0.63844312465104458</v>
       </c>
       <c r="O9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.73704163933552791</v>
+      </c>
+      <c r="P9">
+        <v>0.62864355497013025</v>
+      </c>
+      <c r="Q9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -1384,28 +1444,34 @@
         <v>0.82380808439287223</v>
       </c>
       <c r="I10">
-        <v>0.74687644612997395</v>
+        <v>0.92990198388035694</v>
       </c>
       <c r="J10">
-        <v>0.67774323753046106</v>
+        <v>0.88149878624692701</v>
       </c>
       <c r="K10">
-        <v>0.6169898824741199</v>
+        <v>0.81845652657482071</v>
       </c>
       <c r="L10">
-        <v>0.43454948848599595</v>
+        <v>0.95663219121242504</v>
       </c>
       <c r="M10">
-        <v>0.32968722147366797</v>
+        <v>0.75477821460341243</v>
       </c>
       <c r="N10">
-        <v>0.24141853348945025</v>
+        <v>0.64396175718332849</v>
       </c>
       <c r="O10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.76966341269542027</v>
+      </c>
+      <c r="P10">
+        <v>0.72183382968779153</v>
+      </c>
+      <c r="Q10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -1419,28 +1485,34 @@
         <v>0.96473221499795514</v>
       </c>
       <c r="I11">
-        <v>0.95089202072768864</v>
+        <v>0.9893985902965784</v>
       </c>
       <c r="J11">
-        <v>0.94550859850655788</v>
+        <v>0.98400878548180459</v>
       </c>
       <c r="K11">
-        <v>0.94123449958851146</v>
+        <v>0.97727267471279466</v>
       </c>
       <c r="L11">
-        <v>0.90480240432274961</v>
+        <v>0.9943645417334972</v>
       </c>
       <c r="M11">
-        <v>0.88439221937246448</v>
+        <v>0.9688840488296192</v>
       </c>
       <c r="N11">
-        <v>0.86412279248543922</v>
+        <v>0.95101729696572601</v>
       </c>
       <c r="O11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.97316620934993392</v>
+      </c>
+      <c r="P11">
+        <v>0.9728181507019803</v>
+      </c>
+      <c r="Q11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>31</v>
       </c>
@@ -1454,28 +1526,34 @@
         <v>0.99949823784361513</v>
       </c>
       <c r="I12">
-        <v>0.9998631058203904</v>
+        <v>0.99953836028545895</v>
       </c>
       <c r="J12">
-        <v>0.99996937567896649</v>
+        <v>0.99976191378450807</v>
       </c>
       <c r="K12">
-        <v>0.99998894100102931</v>
+        <v>0.99991027304056324</v>
       </c>
       <c r="L12">
-        <v>0.99999605032943084</v>
+        <v>0.99985295591252965</v>
       </c>
       <c r="M12">
-        <v>0.99999913917170424</v>
+        <v>0.99986737008753213</v>
       </c>
       <c r="N12">
-        <v>0.99999967264258616</v>
+        <v>0.99995123491289428</v>
       </c>
       <c r="O12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.99996492287824645</v>
+      </c>
+      <c r="P12">
+        <v>0.99998596885599533</v>
+      </c>
+      <c r="Q12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>33</v>
       </c>
@@ -1489,28 +1567,34 @@
         <v>0.77795349091178134</v>
       </c>
       <c r="I13">
-        <v>0.68061648198912972</v>
+        <v>0.86528712018247023</v>
       </c>
       <c r="J13">
-        <v>0.57595497562787812</v>
+        <v>0.81640688775896919</v>
       </c>
       <c r="K13">
-        <v>0.50462681261046749</v>
+        <v>0.68754803215679694</v>
       </c>
       <c r="L13">
-        <v>0.29916799468642741</v>
+        <v>0.91788807456749966</v>
       </c>
       <c r="M13">
-        <v>0.20220657717920423</v>
+        <v>0.7170179545898222</v>
       </c>
       <c r="N13">
-        <v>0.11830828867350776</v>
+        <v>0.53525641009329183</v>
       </c>
       <c r="O13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.61097560960023978</v>
+      </c>
+      <c r="P13">
+        <v>0.51548260640163279</v>
+      </c>
+      <c r="Q13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>35</v>
       </c>
@@ -1524,28 +1608,34 @@
         <v>0.99997439477390471</v>
       </c>
       <c r="I14">
-        <v>0.99999617384840256</v>
+        <v>0.99996857558720786</v>
       </c>
       <c r="J14">
-        <v>0.99999969564596014</v>
+        <v>0.9999893834234167</v>
       </c>
       <c r="K14">
-        <v>0.99999995849716539</v>
+        <v>0.99999904569176046</v>
       </c>
       <c r="L14">
-        <v>0.99999999522955907</v>
+        <v>0.9999978687141069</v>
       </c>
       <c r="M14">
-        <v>0.99999999932652606</v>
+        <v>0.99999888517239954</v>
       </c>
       <c r="N14">
-        <v>0.9999999997755088</v>
+        <v>0.99999983881995225</v>
       </c>
       <c r="O14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.99999989695045532</v>
+      </c>
+      <c r="P14">
+        <v>0.99999997737936641</v>
+      </c>
+      <c r="Q14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>37</v>
       </c>
@@ -1559,28 +1649,34 @@
         <v>0.86775841574123669</v>
       </c>
       <c r="I15">
-        <v>0.75357204384146526</v>
+        <v>0.94177885592544563</v>
       </c>
       <c r="J15">
-        <v>0.61199321009554142</v>
+        <v>0.88489277476509309</v>
       </c>
       <c r="K15">
-        <v>0.43594109924350827</v>
+        <v>0.76715297446927488</v>
       </c>
       <c r="L15">
-        <v>0.24757794643949929</v>
+        <v>0.95752352931660534</v>
       </c>
       <c r="M15">
-        <v>0.12568758316830175</v>
+        <v>0.69807179910697548</v>
       </c>
       <c r="N15">
-        <v>7.0206960124385612E-2</v>
+        <v>0.4951707716618991</v>
       </c>
       <c r="O15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.56479422899518372</v>
+      </c>
+      <c r="P15">
+        <v>0.43602740101290227</v>
+      </c>
+      <c r="Q15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>39</v>
       </c>
@@ -1594,28 +1690,34 @@
         <v>0.9999898678152469</v>
       </c>
       <c r="I16">
-        <v>0.99999849892263615</v>
+        <v>0.99998708150043525</v>
       </c>
       <c r="J16">
-        <v>0.99999989016491819</v>
+        <v>0.99999685763154778</v>
       </c>
       <c r="K16">
-        <v>0.99999998372813459</v>
+        <v>0.99999951655741426</v>
       </c>
       <c r="L16">
-        <v>0.99999999749663604</v>
+        <v>0.9999989295206172</v>
       </c>
       <c r="M16">
-        <v>0.99999999961486707</v>
+        <v>0.99999940125701203</v>
       </c>
       <c r="N16">
-        <v>0.99999999990756816</v>
+        <v>0.99999988025134512</v>
       </c>
       <c r="O16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.99999990962365415</v>
+      </c>
+      <c r="P16">
+        <v>0.99999997978423705</v>
+      </c>
+      <c r="Q16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>41</v>
       </c>
@@ -1629,28 +1731,34 @@
         <v>0.99999800668358985</v>
       </c>
       <c r="I17">
-        <v>0.9999997981448121</v>
+        <v>0.99999767867025846</v>
       </c>
       <c r="J17">
-        <v>0.99999997253670436</v>
+        <v>0.99999944889196346</v>
       </c>
       <c r="K17">
-        <v>0.99999999443052034</v>
+        <v>0.99999996779237077</v>
       </c>
       <c r="L17">
-        <v>0.99999999945038032</v>
+        <v>0.99999992270169336</v>
       </c>
       <c r="M17">
-        <v>0.99999999994289657</v>
+        <v>0.99999996476106456</v>
       </c>
       <c r="N17">
-        <v>0.99999999998857925</v>
+        <v>0.99999999635459269</v>
       </c>
       <c r="O17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.99999999793098504</v>
+      </c>
+      <c r="P17">
+        <v>0.99999999963405173</v>
+      </c>
+      <c r="Q17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>43</v>
       </c>
@@ -1664,28 +1772,34 @@
         <v>0.99915984598870045</v>
       </c>
       <c r="I18">
-        <v>0.99976289046248434</v>
+        <v>0.99896909873972994</v>
       </c>
       <c r="J18">
-        <v>0.99992853049210217</v>
+        <v>0.99959319340116493</v>
       </c>
       <c r="K18">
-        <v>0.99997617569555997</v>
+        <v>0.99988755981114308</v>
       </c>
       <c r="L18">
-        <v>0.99999301141970554</v>
+        <v>0.99970854059130776</v>
       </c>
       <c r="M18">
-        <v>0.99999829764451897</v>
+        <v>0.99989068280828786</v>
       </c>
       <c r="N18">
-        <v>0.99999951984786728</v>
+        <v>0.99996095540194474</v>
       </c>
       <c r="O18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.99996095540194474</v>
+      </c>
+      <c r="P18">
+        <v>0.99999084111685732</v>
+      </c>
+      <c r="Q18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>45</v>
       </c>
@@ -1708,28 +1822,34 @@
         <v>0.99</v>
       </c>
       <c r="I19">
-        <v>0.99899759422614265</v>
+        <v>0.98937381404174574</v>
       </c>
       <c r="J19">
-        <v>0.99977792004508981</v>
+        <v>0.99788776664850598</v>
       </c>
       <c r="K19">
-        <v>0.9999562246119521</v>
+        <v>0.99968651247932239</v>
       </c>
       <c r="L19">
-        <v>0.99999297011732358</v>
+        <v>0.99918534106289492</v>
       </c>
       <c r="M19">
-        <v>0.99999900986969925</v>
+        <v>0.99964342331530109</v>
       </c>
       <c r="N19">
-        <v>0.99999979041021059</v>
+        <v>0.99994595687884935</v>
       </c>
       <c r="O19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.99996250007105481</v>
+      </c>
+      <c r="P19">
+        <v>0.99999266283606958</v>
+      </c>
+      <c r="Q19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>47</v>
       </c>
@@ -1743,28 +1863,34 @@
         <v>0.87128833271883765</v>
       </c>
       <c r="I20">
-        <v>0.81112490678226834</v>
+        <v>0.9417046252579141</v>
       </c>
       <c r="J20">
-        <v>0.76235419527201753</v>
+        <v>0.92238083865143883</v>
       </c>
       <c r="K20">
-        <v>0.71040790073213878</v>
+        <v>0.87410488372453388</v>
       </c>
       <c r="L20">
-        <v>0.57574126425625027</v>
+        <v>0.96524456641703471</v>
       </c>
       <c r="M20">
-        <v>0.47357862018437319</v>
+        <v>0.88882845767558794</v>
       </c>
       <c r="N20">
-        <v>0.38905512327503439</v>
+        <v>0.81003246866093648</v>
       </c>
       <c r="O20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.87664619399320654</v>
+      </c>
+      <c r="P20">
+        <v>0.85997626823064277</v>
+      </c>
+      <c r="Q20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>49</v>
       </c>
@@ -1778,28 +1904,34 @@
         <v>0.99999062954791906</v>
       </c>
       <c r="I21">
-        <v>0.99999833127650339</v>
+        <v>0.99999177481597545</v>
       </c>
       <c r="J21">
-        <v>0.99999979840894626</v>
+        <v>0.99999823744917538</v>
       </c>
       <c r="K21">
-        <v>0.99</v>
+        <v>0.99999969123152344</v>
       </c>
       <c r="L21">
-        <v>0.99785073741940267</v>
+        <v>0.99999944421687947</v>
       </c>
       <c r="M21">
-        <v>0.99960578090411067</v>
+        <v>0.99999962319781699</v>
       </c>
       <c r="N21">
-        <v>0.99992002833716465</v>
+        <v>0.99999993251302088</v>
       </c>
       <c r="O21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.99999996654993095</v>
+      </c>
+      <c r="P21">
+        <v>0.99999999400205641</v>
+      </c>
+      <c r="Q21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>51</v>
       </c>
@@ -1813,28 +1945,34 @@
         <v>0.99997200084585958</v>
       </c>
       <c r="I22">
-        <v>0.999995205513036</v>
+        <v>0.99996733447260411</v>
       </c>
       <c r="J22">
-        <v>0.99999888248389168</v>
+        <v>0.99998987092602021</v>
       </c>
       <c r="K22">
-        <v>0.9999997081112233</v>
+        <v>0.99999812423007794</v>
       </c>
       <c r="L22">
-        <v>0.99999995945988185</v>
+        <v>0.99999441737211658</v>
       </c>
       <c r="M22">
-        <v>0.99999999384908533</v>
+        <v>0.9999976536705425</v>
       </c>
       <c r="N22">
-        <v>0.99999999894676117</v>
+        <v>0.99999959727102672</v>
       </c>
       <c r="O22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.99999972088087519</v>
+      </c>
+      <c r="P22">
+        <v>0.99999992235030299</v>
+      </c>
+      <c r="Q22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>53</v>
       </c>
@@ -1848,28 +1986,34 @@
         <v>0.9999942176104234</v>
       </c>
       <c r="I23">
-        <v>0.99999938320859239</v>
+        <v>0.99999414622331562</v>
       </c>
       <c r="J23">
-        <v>0.99999986816665809</v>
+        <v>0.99999852537804179</v>
       </c>
       <c r="K23">
-        <v>0.9999999740182437</v>
+        <v>0.99999981834343699</v>
       </c>
       <c r="L23">
-        <v>0.99999999560602637</v>
+        <v>0.99999965615013298</v>
       </c>
       <c r="M23">
-        <v>0.99999999955163532</v>
+        <v>0.99999977493460579</v>
       </c>
       <c r="N23">
-        <v>0.99999999992050281</v>
+        <v>0.99999996248909395</v>
       </c>
       <c r="O23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.99999998141351465</v>
+      </c>
+      <c r="P23">
+        <v>0.99999999652339111</v>
+      </c>
+      <c r="Q23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>55</v>
       </c>
@@ -1883,28 +2027,34 @@
         <v>0.99999939557647632</v>
       </c>
       <c r="I24">
-        <v>0.99999994761659905</v>
+        <v>0.99999929756191974</v>
       </c>
       <c r="J24">
-        <v>0.99999999523787231</v>
+        <v>0.99999982575170199</v>
       </c>
       <c r="K24">
-        <v>0.99999999916575866</v>
+        <v>0.99</v>
       </c>
       <c r="L24">
-        <v>0.99999999995490596</v>
+        <v>0.97578744375401749</v>
       </c>
       <c r="M24">
-        <v>0.99999999999564615</v>
+        <v>0.98937401708847417</v>
       </c>
       <c r="N24">
-        <v>0.99999999999924827</v>
+        <v>0.99954956911481874</v>
       </c>
       <c r="O24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.99975114038322654</v>
+      </c>
+      <c r="P24">
+        <v>0.99995021816569485</v>
+      </c>
+      <c r="Q24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>57</v>
       </c>
@@ -1918,28 +2068,34 @@
         <v>0.9999968580190568</v>
       </c>
       <c r="I25">
-        <v>0.99999972071200549</v>
+        <v>0.99999643908975611</v>
       </c>
       <c r="J25">
-        <v>0.99999997726725054</v>
+        <v>0.99999895546369999</v>
       </c>
       <c r="K25">
-        <v>0.99999999712574428</v>
+        <v>0.99999991691180534</v>
       </c>
       <c r="L25">
-        <v>0.99999999969920572</v>
+        <v>0.99999982846309721</v>
       </c>
       <c r="M25">
-        <v>0.99999999996152633</v>
+        <v>0.9999999115512771</v>
       </c>
       <c r="N25">
-        <v>0.999999999990135</v>
+        <v>0.99999998813492652</v>
       </c>
       <c r="O25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.99999999181719079</v>
+      </c>
+      <c r="P25">
+        <v>0.99999999828262032</v>
+      </c>
+      <c r="Q25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>59</v>
       </c>
@@ -1953,28 +2109,34 @@
         <v>0.99999778661572813</v>
       </c>
       <c r="I26">
-        <v>0.99999974460900698</v>
+        <v>0.99999716686988782</v>
       </c>
       <c r="J26">
-        <v>0.99999996914738987</v>
+        <v>0.99999937711186104</v>
       </c>
       <c r="K26">
-        <v>0.99999999475295742</v>
+        <v>0.99999996359742505</v>
       </c>
       <c r="L26">
-        <v>0.99999999959377739</v>
+        <v>0.99999988546507801</v>
       </c>
       <c r="M26">
-        <v>0.99999999993961564</v>
+        <v>0.99999995704940114</v>
       </c>
       <c r="N26">
-        <v>0.99999999999080236</v>
+        <v>0.99999999682915031</v>
       </c>
       <c r="O26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.99999999810912632</v>
+      </c>
+      <c r="P26">
+        <v>0.99999999963486585</v>
+      </c>
+      <c r="Q26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>61</v>
       </c>
@@ -1988,28 +2150,34 @@
         <v>0.99998231116460623</v>
       </c>
       <c r="I27">
-        <v>0.99999695015614742</v>
+        <v>0.99998592496183236</v>
       </c>
       <c r="J27">
-        <v>0.99999957344729329</v>
+        <v>0.9999969401753892</v>
       </c>
       <c r="K27">
-        <v>0.99999995509969797</v>
+        <v>0.99999948252834581</v>
       </c>
       <c r="L27">
-        <v>0.9999999914787745</v>
+        <v>0.9999991319833359</v>
       </c>
       <c r="M27">
-        <v>0.99999999869814604</v>
+        <v>0.99999942622610394</v>
       </c>
       <c r="N27">
-        <v>0.99999999970965847</v>
+        <v>0.99999987448690397</v>
       </c>
       <c r="O27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.99999994620866917</v>
+      </c>
+      <c r="P27">
+        <v>0.99999999358778802</v>
+      </c>
+      <c r="Q27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>63</v>
       </c>
@@ -2023,28 +2191,34 @@
         <v>0.99762416956911526</v>
       </c>
       <c r="I28">
-        <v>0.99865016890364033</v>
+        <v>0.99898889078805397</v>
       </c>
       <c r="J28">
-        <v>0.99937199335101601</v>
+        <v>0.99919936988960933</v>
       </c>
       <c r="K28">
-        <v>0.99968862851732998</v>
+        <v>0.99955758862692967</v>
       </c>
       <c r="L28">
-        <v>0.99981611910569512</v>
+        <v>0.99967492491733856</v>
       </c>
       <c r="M28">
-        <v>0.99990966409191373</v>
+        <v>0.9994057370551962</v>
       </c>
       <c r="N28">
-        <v>0.99994479278337178</v>
+        <v>0.99964335745733868</v>
       </c>
       <c r="O28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.99</v>
+      </c>
+      <c r="P28">
+        <v>0.99438964799565654</v>
+      </c>
+      <c r="Q28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>65</v>
       </c>
@@ -2058,28 +2232,34 @@
         <v>0.99993865266796289</v>
       </c>
       <c r="I29">
-        <v>0.99998626486870945</v>
+        <v>0.99991820522991415</v>
       </c>
       <c r="J29">
-        <v>0.99999688810125853</v>
+        <v>0.9999766287002253</v>
       </c>
       <c r="K29">
-        <v>0.99999914238817733</v>
+        <v>0.9999956517684877</v>
       </c>
       <c r="L29">
-        <v>0.99999991188912851</v>
+        <v>0.99998695541890481</v>
       </c>
       <c r="M29">
-        <v>0.99999998368317067</v>
+        <v>0.99999478212672288</v>
       </c>
       <c r="N29">
-        <v>0.99999999706531839</v>
+        <v>0.99999921535392344</v>
       </c>
       <c r="O29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.99999933878131453</v>
+      </c>
+      <c r="P29">
+        <v>0.99999979369967629</v>
+      </c>
+      <c r="Q29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>67</v>
       </c>
@@ -2093,28 +2273,34 @@
         <v>0.99999551151806954</v>
       </c>
       <c r="I30">
-        <v>0.99999946138004092</v>
+        <v>0.99999405751143677</v>
       </c>
       <c r="J30">
-        <v>0.99999992359997059</v>
+        <v>0.99999852554136248</v>
       </c>
       <c r="K30">
-        <v>0.99999998515970556</v>
+        <v>0.99999988891049918</v>
       </c>
       <c r="L30">
-        <v>0.99999999901719905</v>
+        <v>0.99999971503133012</v>
       </c>
       <c r="M30">
-        <v>0.99999999989516797</v>
+        <v>0.99999987478647356</v>
       </c>
       <c r="N30">
-        <v>0.99999999998420341</v>
+        <v>0.99999999222812508</v>
       </c>
       <c r="O30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.99999999579320531</v>
+      </c>
+      <c r="P30">
+        <v>0.99999999900283387</v>
+      </c>
+      <c r="Q30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>69</v>
       </c>
@@ -2128,28 +2314,34 @@
         <v>0.99999460333573698</v>
       </c>
       <c r="I31">
-        <v>0.9999992991312201</v>
+        <v>0.99999414264758368</v>
       </c>
       <c r="J31">
-        <v>0.99999994083571442</v>
+        <v>0.99999871220741388</v>
       </c>
       <c r="K31">
-        <v>0.99999999040579102</v>
+        <v>0.99999988839117793</v>
       </c>
       <c r="L31">
-        <v>0.9999999991900993</v>
+        <v>0.99999973957945387</v>
       </c>
       <c r="M31">
-        <v>0.99999999992731659</v>
+        <v>0.99999986378000505</v>
       </c>
       <c r="N31">
-        <v>0.99999999998665001</v>
+        <v>0.99999998164411197</v>
       </c>
       <c r="O31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.99999999105738779</v>
+      </c>
+      <c r="P31">
+        <v>0.99999999812392748</v>
+      </c>
+      <c r="Q31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>71</v>
       </c>
@@ -2163,28 +2355,34 @@
         <v>0.99999737430762625</v>
       </c>
       <c r="I32">
-        <v>0.99999973241288509</v>
+        <v>0.9999974950288123</v>
       </c>
       <c r="J32">
-        <v>0.99999997914905081</v>
+        <v>0.99999948842035735</v>
       </c>
       <c r="K32">
-        <v>0.99999999723828492</v>
+        <v>0.99999995536551367</v>
       </c>
       <c r="L32">
-        <v>0.99999999972565745</v>
+        <v>0.99999990667335137</v>
       </c>
       <c r="M32">
-        <v>0.99999999997327826</v>
+        <v>0.99999994581033091</v>
       </c>
       <c r="N32">
-        <v>0.99999999999505829</v>
+        <v>0.9999999926456874</v>
       </c>
       <c r="O32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.99999999638624304</v>
+      </c>
+      <c r="P32">
+        <v>0.99999999952450569</v>
+      </c>
+      <c r="Q32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>73</v>
       </c>
@@ -2198,28 +2396,34 @@
         <v>0.99999920693713185</v>
       </c>
       <c r="I33">
-        <v>0.99999990419368068</v>
+        <v>0.99999903546424462</v>
       </c>
       <c r="J33">
-        <v>0.99999999015688423</v>
+        <v>0.99999977686096575</v>
       </c>
       <c r="K33">
-        <v>0.99999999790110028</v>
+        <v>0.99999998793842804</v>
       </c>
       <c r="L33">
-        <v>0.99</v>
+        <v>0.99999996710480443</v>
       </c>
       <c r="M33">
-        <v>0.99890177774727162</v>
+        <v>0.99999998576178073</v>
       </c>
       <c r="N33">
-        <v>0.99985044010336466</v>
+        <v>0.99999999867787959</v>
       </c>
       <c r="O33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.99999999921931926</v>
+      </c>
+      <c r="P33">
+        <v>0.9999999998135688</v>
+      </c>
+      <c r="Q33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>75</v>
       </c>
@@ -2230,28 +2434,34 @@
         <v>0.99997414158921138</v>
       </c>
       <c r="I34">
-        <v>0.999996069435371</v>
+        <v>0.99997144004136185</v>
       </c>
       <c r="J34">
-        <v>0.99999920698885858</v>
+        <v>0.99999359848811198</v>
       </c>
       <c r="K34">
-        <v>0.99999981381466252</v>
+        <v>0.99999900665657626</v>
       </c>
       <c r="L34">
-        <v>0.99999996817344172</v>
+        <v>0.99999713034660465</v>
       </c>
       <c r="M34">
-        <v>0.99999999530427819</v>
+        <v>0.99999841253012878</v>
       </c>
       <c r="N34">
-        <v>0.99999999919829141</v>
+        <v>0.99999971396902032</v>
       </c>
       <c r="O34">
+        <v>0.9999997956921407</v>
+      </c>
+      <c r="P34">
+        <v>0.99999995459824631</v>
+      </c>
+      <c r="Q34">
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>77</v>
       </c>
@@ -2265,28 +2475,34 @@
         <v>0.96084285259125757</v>
       </c>
       <c r="I35">
-        <v>0.95255411880352547</v>
+        <v>0.98765670043697262</v>
       </c>
       <c r="J35">
-        <v>0.94086267485996278</v>
+        <v>0.9863614924179992</v>
       </c>
       <c r="K35">
-        <v>0.93624873769222483</v>
+        <v>0.97609189834880727</v>
       </c>
       <c r="L35">
-        <v>0.88334723639912205</v>
+        <v>0.99367821929560263</v>
       </c>
       <c r="M35">
-        <v>0.84162179535670767</v>
+        <v>0.96281008574098859</v>
       </c>
       <c r="N35">
-        <v>0.78690668273703424</v>
+        <v>0.93789561606571248</v>
       </c>
       <c r="O35">
+        <v>0.97366596605361089</v>
+      </c>
+      <c r="P35">
+        <v>0.9692270689171546</v>
+      </c>
+      <c r="Q35">
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>79</v>
       </c>
@@ -2300,28 +2516,34 @@
         <v>0.9999981753482331</v>
       </c>
       <c r="I36">
-        <v>0.99999981164854168</v>
+        <v>0.99999794438012979</v>
       </c>
       <c r="J36">
-        <v>0.99999997821785491</v>
+        <v>0.99999959179112641</v>
       </c>
       <c r="K36">
-        <v>0.99999999724092825</v>
+        <v>0.99999996438444749</v>
       </c>
       <c r="L36">
-        <v>0.99999999965984043</v>
+        <v>0.9999999004383483</v>
       </c>
       <c r="M36">
-        <v>0.99999999995918087</v>
+        <v>0.99999995251674823</v>
       </c>
       <c r="N36">
-        <v>0.99999999999234634</v>
+        <v>0.99999999571331732</v>
       </c>
       <c r="O36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.99999999737137379</v>
+      </c>
+      <c r="P36">
+        <v>0.99999999956789709</v>
+      </c>
+      <c r="Q36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>81</v>
       </c>
@@ -2335,28 +2557,34 @@
         <v>0.93386328480232839</v>
       </c>
       <c r="I37">
-        <v>0.92380923157957573</v>
+        <v>0.98038951183387391</v>
       </c>
       <c r="J37">
-        <v>0.91664615721161857</v>
+        <v>0.97313236787366209</v>
       </c>
       <c r="K37">
-        <v>0.9100903952106405</v>
+        <v>0.96486684434691006</v>
       </c>
       <c r="L37">
-        <v>0.86627906547755051</v>
+        <v>0.98791329605057299</v>
       </c>
       <c r="M37">
-        <v>0.84715350624371377</v>
+        <v>0.95557402315556905</v>
       </c>
       <c r="N37">
-        <v>0.805015233679238</v>
+        <v>0.93544435278313287</v>
       </c>
       <c r="O37">
+        <v>0.96913209488845098</v>
+      </c>
+      <c r="P37">
+        <v>0.96618649951195767</v>
+      </c>
+      <c r="Q37">
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>83</v>
       </c>
@@ -2373,28 +2601,34 @@
         <v>0.99</v>
       </c>
       <c r="I38">
-        <v>0.99847543098393343</v>
+        <v>0.98747390396659707</v>
       </c>
       <c r="J38">
-        <v>0.99985961540019064</v>
+        <v>0.99655238460065121</v>
       </c>
       <c r="K38">
-        <v>0.99998063426325801</v>
+        <v>0.99968559501144094</v>
       </c>
       <c r="L38">
-        <v>0.99999872311513938</v>
+        <v>0.99927391519257225</v>
       </c>
       <c r="M38">
-        <v>0.99999978199503681</v>
+        <v>0.99964782715321643</v>
       </c>
       <c r="N38">
-        <v>0.99999996107053535</v>
+        <v>0.9999672292677988</v>
       </c>
       <c r="O38">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.99997269090734264</v>
+      </c>
+      <c r="P38">
+        <v>0.99999219724989363</v>
+      </c>
+      <c r="Q38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>85</v>
       </c>
@@ -2408,28 +2642,34 @@
         <v>0.99998993039250639</v>
       </c>
       <c r="I39">
-        <v>0.99999837803609792</v>
+        <v>0.99998629419519358</v>
       </c>
       <c r="J39">
-        <v>0.9999997521996189</v>
+        <v>0.99999743013298092</v>
       </c>
       <c r="K39">
-        <v>0.99999995756841908</v>
+        <v>0.99999969870456262</v>
       </c>
       <c r="L39">
-        <v>0.99999999451564581</v>
+        <v>0.99999905937094324</v>
       </c>
       <c r="M39">
-        <v>0.9999999990922448</v>
+        <v>0.99999961031060469</v>
       </c>
       <c r="N39">
-        <v>0.99999999984666299</v>
+        <v>0.99999995334702829</v>
       </c>
       <c r="O39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.99999996752587217</v>
+      </c>
+      <c r="P39">
+        <v>0.99999999421693608</v>
+      </c>
+      <c r="Q39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>87</v>
       </c>
@@ -2443,28 +2683,34 @@
         <v>0.99999275108747965</v>
       </c>
       <c r="I40">
-        <v>0.99999899186680163</v>
+        <v>0.99999069398279983</v>
       </c>
       <c r="J40">
-        <v>0.99999987655500933</v>
+        <v>0.99999808598231388</v>
       </c>
       <c r="K40">
-        <v>0.99999997771131877</v>
+        <v>0.99999987324363537</v>
       </c>
       <c r="L40">
-        <v>0.99999999825186814</v>
+        <v>0.99999963152228488</v>
       </c>
       <c r="M40">
-        <v>0.99999999977708387</v>
+        <v>0.99999984513252138</v>
       </c>
       <c r="N40">
-        <v>0.99999999994904776</v>
+        <v>0.99999998494343745</v>
       </c>
       <c r="O40">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.99999999129758299</v>
+      </c>
+      <c r="P40">
+        <v>0.99999999791898719</v>
+      </c>
+      <c r="Q40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>89</v>
       </c>
@@ -2475,28 +2721,34 @@
         <v>0.99999460710773957</v>
       </c>
       <c r="I41">
-        <v>0.9999992701314786</v>
+        <v>0.99999329974867857</v>
       </c>
       <c r="J41">
-        <v>0.9999998890599161</v>
+        <v>0.99999801904678232</v>
       </c>
       <c r="K41">
-        <v>0.99999997654924855</v>
+        <v>0.99999979722490062</v>
       </c>
       <c r="L41">
-        <v>0.99999999808919793</v>
+        <v>0.99999957755196911</v>
       </c>
       <c r="M41">
-        <v>0.99999999971636533</v>
+        <v>0.99999976722246953</v>
       </c>
       <c r="N41">
-        <v>0.99999999996871669</v>
+        <v>0.99999997350499104</v>
       </c>
       <c r="O41">
+        <v>0.99999998482056762</v>
+      </c>
+      <c r="P41">
+        <v>0.99999999604569401</v>
+      </c>
+      <c r="Q41">
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>91</v>
       </c>
@@ -2510,28 +2762,34 @@
         <v>0.99997381908143268</v>
       </c>
       <c r="I42">
-        <v>0.99999525697828884</v>
+        <v>0.99996271243922585</v>
       </c>
       <c r="J42">
-        <v>0.99999926219366764</v>
+        <v>0.99999110809839864</v>
       </c>
       <c r="K42">
-        <v>0.99999985133744251</v>
+        <v>0.99999910440562689</v>
       </c>
       <c r="L42">
-        <v>0.99999998648522026</v>
+        <v>0.99999733561145276</v>
       </c>
       <c r="M42">
-        <v>0.99999999816585128</v>
+        <v>0.99999893424287745</v>
       </c>
       <c r="N42">
-        <v>0.9999999995692529</v>
+        <v>0.99999985683846337</v>
       </c>
       <c r="O42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.9999999121186558</v>
+      </c>
+      <c r="P42">
+        <v>0.99999997836766763</v>
+      </c>
+      <c r="Q42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>93</v>
       </c>
@@ -2542,28 +2800,34 @@
         <v>0.99992813525226121</v>
       </c>
       <c r="I43">
-        <v>0.99998039949891848</v>
+        <v>0.99993388405196781</v>
       </c>
       <c r="J43">
-        <v>0.99999355975060311</v>
+        <v>0.99997449709855357</v>
       </c>
       <c r="K43">
-        <v>0.99999791126137672</v>
+        <v>0.99999319909908968</v>
       </c>
       <c r="L43">
-        <v>0.99999944300218069</v>
+        <v>0.99998595953202707</v>
       </c>
       <c r="M43">
-        <v>0.99999986979266198</v>
+        <v>0.99999134166481596</v>
       </c>
       <c r="N43">
-        <v>0.99999997267253127</v>
+        <v>0.99999681677110674</v>
       </c>
       <c r="O43">
+        <v>0.99999761257643016</v>
+      </c>
+      <c r="P43">
+        <v>0.99999938783902353</v>
+      </c>
+      <c r="Q43">
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>95</v>
       </c>
@@ -2577,28 +2841,34 @@
         <v>0.88878503398316033</v>
       </c>
       <c r="I44">
-        <v>0.8677514679532724</v>
+        <v>0.95214725352757901</v>
       </c>
       <c r="J44">
-        <v>0.8562838944788338</v>
+        <v>0.93238814860806218</v>
       </c>
       <c r="K44">
-        <v>0.84893416483940121</v>
+        <v>0.90676681824761518</v>
       </c>
       <c r="L44">
-        <v>0.78763870768539368</v>
+        <v>0.97219154821800302</v>
       </c>
       <c r="M44">
-        <v>0.73824401686749419</v>
+        <v>0.88721039568716487</v>
       </c>
       <c r="N44">
-        <v>0.65171297399772055</v>
+        <v>0.84807901093166371</v>
       </c>
       <c r="O44">
+        <v>0.90049953405937311</v>
+      </c>
+      <c r="P44">
+        <v>0.88003016514347077</v>
+      </c>
+      <c r="Q44">
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>97</v>
       </c>
@@ -2612,28 +2882,34 @@
         <v>0.99998843114814306</v>
       </c>
       <c r="I45">
-        <v>0.99999874079225803</v>
+        <v>0.99998813826929167</v>
       </c>
       <c r="J45">
-        <v>0.99999978224204333</v>
+        <v>0.99999739398958742</v>
       </c>
       <c r="K45">
-        <v>0.9999999599709567</v>
+        <v>0.99999969340983474</v>
       </c>
       <c r="L45">
-        <v>0.9999999941133757</v>
+        <v>0.99999914592786443</v>
       </c>
       <c r="M45">
-        <v>0.99999999915300364</v>
+        <v>0.99999960796670739</v>
       </c>
       <c r="N45">
-        <v>0.99999999980894827</v>
+        <v>0.9999999361806059</v>
       </c>
       <c r="O45">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.99999996474738129</v>
+      </c>
+      <c r="P45">
+        <v>0.99999999386910954</v>
+      </c>
+      <c r="Q45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>99</v>
       </c>
@@ -2647,28 +2923,34 @@
         <v>0.99206997833515809</v>
       </c>
       <c r="I46">
-        <v>0.99216146510159153</v>
+        <v>0.99</v>
       </c>
       <c r="J46">
-        <v>0.9925319411138871</v>
+        <v>0.98888750156074412</v>
       </c>
       <c r="K46">
-        <v>0.99343871497004888</v>
+        <v>0.98710870524510974</v>
       </c>
       <c r="L46">
-        <v>0.9920313635031095</v>
+        <v>0.99433955484343084</v>
       </c>
       <c r="M46">
-        <v>0.99174223545288009</v>
+        <v>0.98545588386755756</v>
       </c>
       <c r="N46">
-        <v>0.99220777057510923</v>
+        <v>0.98330090211893995</v>
       </c>
       <c r="O46">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.99283407633565901</v>
+      </c>
+      <c r="P46">
+        <v>0.99433414424608324</v>
+      </c>
+      <c r="Q46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>101</v>
       </c>
@@ -2682,28 +2964,34 @@
         <v>0.99999973361658001</v>
       </c>
       <c r="I47">
-        <v>0.99999997578331956</v>
+        <v>0.99999970442388508</v>
       </c>
       <c r="J47">
-        <v>0.99999999728917743</v>
+        <v>0.99999994810494419</v>
       </c>
       <c r="K47">
-        <v>0.99999999947464668</v>
+        <v>0.99999999656576821</v>
       </c>
       <c r="L47">
-        <v>0.99999999997795719</v>
+        <v>0.99999999183416011</v>
       </c>
       <c r="M47">
-        <v>0.99999999999828038</v>
+        <v>0.99999999656175154</v>
       </c>
       <c r="N47">
-        <v>0.99999999999981715</v>
+        <v>0.99999999959390762</v>
       </c>
       <c r="O47">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.99999999975299525</v>
+      </c>
+      <c r="P47">
+        <v>0.9999999999612903</v>
+      </c>
+      <c r="Q47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>103</v>
       </c>
@@ -2717,28 +3005,34 @@
         <v>0.99999922358323101</v>
       </c>
       <c r="I48">
-        <v>0.99999994092476874</v>
+        <v>0.99999902496518145</v>
       </c>
       <c r="J48">
-        <v>0.99999999456779454</v>
+        <v>0.99999976549778136</v>
       </c>
       <c r="K48">
-        <v>0.99999999925073024</v>
+        <v>0.99999998436651538</v>
       </c>
       <c r="L48">
-        <v>0.99999999993264987</v>
+        <v>0.99999997015425712</v>
       </c>
       <c r="M48">
-        <v>0.9999999999921686</v>
+        <v>0.99999998414444891</v>
       </c>
       <c r="N48">
-        <v>0.99999999999837641</v>
+        <v>0.99999999811243434</v>
       </c>
       <c r="O48">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.99999999887354951</v>
+      </c>
+      <c r="P48">
+        <v>0.99999999978285292</v>
+      </c>
+      <c r="Q48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>105</v>
       </c>
@@ -2752,28 +3046,34 @@
         <v>0.9998216572754155</v>
       </c>
       <c r="I49">
-        <v>0.99994151996556191</v>
+        <v>0.99987342764192921</v>
       </c>
       <c r="J49">
-        <v>0.99998710617627273</v>
+        <v>0.99995347822960301</v>
       </c>
       <c r="K49">
-        <v>0.99999584410314579</v>
+        <v>0.99998596280293317</v>
       </c>
       <c r="L49">
-        <v>0.99999862643704851</v>
+        <v>0.99997861014269773</v>
       </c>
       <c r="M49">
-        <v>0.99999966733987644</v>
+        <v>0.99998117687725918</v>
       </c>
       <c r="N49">
-        <v>0.99999991811441058</v>
+        <v>0.99999361350392879</v>
       </c>
       <c r="O49">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.9999972306244298</v>
+      </c>
+      <c r="P49">
+        <v>0.99999923072746966</v>
+      </c>
+      <c r="Q49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>107</v>
       </c>
@@ -2799,28 +3099,34 @@
         <v>0.99</v>
       </c>
       <c r="I50">
-        <v>0.9984112730538095</v>
+        <v>0.99</v>
       </c>
       <c r="J50">
-        <v>0.99966760947209776</v>
+        <v>0.99693179136181254</v>
       </c>
       <c r="K50">
-        <v>0.99990537404122914</v>
+        <v>0.99962907327061712</v>
       </c>
       <c r="L50">
-        <v>0.99998890499528847</v>
+        <v>0.99921647836654737</v>
       </c>
       <c r="M50">
-        <v>0.99999824008627192</v>
+        <v>0.99960186726056299</v>
       </c>
       <c r="N50">
-        <v>0.99999976376960942</v>
+        <v>0.99993060557211999</v>
       </c>
       <c r="O50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.99995553255908343</v>
+      </c>
+      <c r="P50">
+        <v>0.99998871684205615</v>
+      </c>
+      <c r="Q50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>109</v>
       </c>
@@ -2834,28 +3140,34 @@
         <v>0.99997216562516167</v>
       </c>
       <c r="I51">
-        <v>0.99999597124457662</v>
+        <v>0.99996907301249449</v>
       </c>
       <c r="J51">
-        <v>0.99999925710648796</v>
+        <v>0.99999209876286455</v>
       </c>
       <c r="K51">
-        <v>0.99999982362949802</v>
+        <v>0.99999870193104201</v>
       </c>
       <c r="L51">
-        <v>0.99999996447212414</v>
+        <v>0.99999762020948468</v>
       </c>
       <c r="M51">
-        <v>0.99999999656181826</v>
+        <v>0.99999857980107165</v>
       </c>
       <c r="N51">
-        <v>0.99999999925465999</v>
+        <v>0.9999997116886129</v>
       </c>
       <c r="O51">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.99999983636378698</v>
+      </c>
+      <c r="P51">
+        <v>0.99999996567072014</v>
+      </c>
+      <c r="Q51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>111</v>
       </c>
@@ -2869,28 +3181,34 @@
         <v>0.99990625813914058</v>
       </c>
       <c r="I52">
-        <v>0.99998582859106588</v>
+        <v>0.99989606986541713</v>
       </c>
       <c r="J52">
-        <v>0.99999730919525964</v>
+        <v>0.99996246718145088</v>
       </c>
       <c r="K52">
-        <v>0.99999936093256303</v>
+        <v>0.99999133833026033</v>
       </c>
       <c r="L52">
-        <v>0.99999985252282664</v>
+        <v>0.99998420530314058</v>
       </c>
       <c r="M52">
-        <v>0.99999997482096736</v>
+        <v>0.99999160900516848</v>
       </c>
       <c r="N52">
-        <v>0.9999999928059905</v>
+        <v>0.99999773214967258</v>
       </c>
       <c r="O52">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.99999846247323143</v>
+      </c>
+      <c r="P52">
+        <v>0.99999970360892976</v>
+      </c>
+      <c r="Q52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>113</v>
       </c>
@@ -2904,28 +3222,34 @@
         <v>0.99994603559665329</v>
       </c>
       <c r="I53">
-        <v>0.99999246973358991</v>
+        <v>0.99994373936825864</v>
       </c>
       <c r="J53">
-        <v>0.99999819272571855</v>
+        <v>0.99997480788965332</v>
       </c>
       <c r="K53">
-        <v>0.99999944576852584</v>
+        <v>0.99999564571735411</v>
       </c>
       <c r="L53">
-        <v>0.99999987043934058</v>
+        <v>0.99999142754220138</v>
       </c>
       <c r="M53">
-        <v>0.9999999762998768</v>
+        <v>0.99999516069124128</v>
       </c>
       <c r="N53">
-        <v>0.99999999313943788</v>
+        <v>0.99999928306241359</v>
       </c>
       <c r="O53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.99999950556017525</v>
+      </c>
+      <c r="P53">
+        <v>0.99999989622863827</v>
+      </c>
+      <c r="Q53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>115</v>
       </c>
@@ -2939,28 +3263,34 @@
         <v>0.99999499169006245</v>
       </c>
       <c r="I54">
-        <v>0.99999934197101414</v>
+        <v>0.99999451144380014</v>
       </c>
       <c r="J54">
-        <v>0.99999992023886475</v>
+        <v>0.99999877055817488</v>
       </c>
       <c r="K54">
-        <v>0.99999998213350461</v>
+        <v>0.99999990825050566</v>
       </c>
       <c r="L54">
-        <v>0.99999999884317659</v>
+        <v>0.99999977688194075</v>
       </c>
       <c r="M54">
-        <v>0.99999999988178445</v>
+        <v>0.99999991152213707</v>
       </c>
       <c r="N54">
-        <v>0.99999999998044553</v>
+        <v>0.99999998946692026</v>
       </c>
       <c r="O54">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.99999999370186976</v>
+      </c>
+      <c r="P54">
+        <v>0.99999999872069234</v>
+      </c>
+      <c r="Q54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>117</v>
       </c>
@@ -2974,28 +3304,34 @@
         <v>0.99763585841249147</v>
       </c>
       <c r="I55">
-        <v>0.99916654533886984</v>
+        <v>0.9982750422887875</v>
       </c>
       <c r="J55">
-        <v>0.99971054417864924</v>
+        <v>0.99932368186916853</v>
       </c>
       <c r="K55">
-        <v>0.99989960520833476</v>
+        <v>0.99974112670881465</v>
       </c>
       <c r="L55">
-        <v>0.99995932037063928</v>
+        <v>0.9996487044409047</v>
       </c>
       <c r="M55">
-        <v>0.99998698215850312</v>
+        <v>0.9996908468755018</v>
       </c>
       <c r="N55">
-        <v>0.99999453027741236</v>
+        <v>0.9998735051589972</v>
       </c>
       <c r="O55">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.99993730829100635</v>
+      </c>
+      <c r="P55">
+        <v>0.99997775365509167</v>
+      </c>
+      <c r="Q55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>119</v>
       </c>
@@ -3021,28 +3357,34 @@
         <v>0.99</v>
       </c>
       <c r="I56">
-        <v>0.99911278695796824</v>
+        <v>0.98694516971279378</v>
       </c>
       <c r="J56">
-        <v>0.99992855675719117</v>
+        <v>0.99661979448350457</v>
       </c>
       <c r="K56">
-        <v>0.99999106903634905</v>
+        <v>0.99989060325739743</v>
       </c>
       <c r="L56">
-        <v>0.99999950928356973</v>
+        <v>0.99979117244144478</v>
       </c>
       <c r="M56">
-        <v>0.99999993649549368</v>
+        <v>0.99989873938124185</v>
       </c>
       <c r="N56">
-        <v>0.99999998588788686</v>
+        <v>0.99999185183519124</v>
       </c>
       <c r="O56">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.99999447580597334</v>
+      </c>
+      <c r="P56">
+        <v>0.99999885473524774</v>
+      </c>
+      <c r="Q56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>121</v>
       </c>
@@ -3056,28 +3398,34 @@
         <v>0.99996014900326502</v>
       </c>
       <c r="I57">
-        <v>0.99999456558613753</v>
+        <v>0.99995306471414191</v>
       </c>
       <c r="J57">
-        <v>0.99999898104290164</v>
+        <v>0.99998328281767512</v>
       </c>
       <c r="K57">
-        <v>0.99999979129777461</v>
+        <v>0.99999741278046372</v>
       </c>
       <c r="L57">
-        <v>0.99999995877486214</v>
+        <v>0.99999598300698977</v>
       </c>
       <c r="M57">
-        <v>0.99999999361991898</v>
+        <v>0.99999760275835281</v>
       </c>
       <c r="N57">
-        <v>0.99999999798523753</v>
+        <v>0.99999961994872832</v>
       </c>
       <c r="O57">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.99999976706531535</v>
+      </c>
+      <c r="P57">
+        <v>0.99999992235509294</v>
+      </c>
+      <c r="Q57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>123</v>
       </c>
@@ -3091,28 +3439,34 @@
         <v>0.99987276773842282</v>
       </c>
       <c r="I58">
-        <v>0.99997419503585128</v>
+        <v>0.99985845613500179</v>
       </c>
       <c r="J58">
-        <v>0.9999940742978406</v>
+        <v>0.99</v>
       </c>
       <c r="K58">
-        <v>0.99999873020076813</v>
+        <v>0.99750058580020307</v>
       </c>
       <c r="L58">
-        <v>0.99999970624018952</v>
+        <v>0.99454578848767583</v>
       </c>
       <c r="M58">
-        <v>0.99999993088002914</v>
+        <v>0.9966845931757764</v>
       </c>
       <c r="N58">
-        <v>0.99999998297044101</v>
+        <v>0.99915590413199951</v>
       </c>
       <c r="O58">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.99933163990450069</v>
+      </c>
+      <c r="P58">
+        <v>0.99982791014588535</v>
+      </c>
+      <c r="Q58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>125</v>
       </c>
@@ -3126,28 +3480,34 @@
         <v>0.99999977243539284</v>
       </c>
       <c r="I59">
-        <v>0.99999996933525959</v>
+        <v>0.99999976356924136</v>
       </c>
       <c r="J59">
-        <v>0.99999999691146491</v>
+        <v>0.99999994684888949</v>
       </c>
       <c r="K59">
-        <v>0.99999999939165207</v>
+        <v>0.99999999660737571</v>
       </c>
       <c r="L59">
-        <v>0.99999999998366851</v>
+        <v>0.99999999155613506</v>
       </c>
       <c r="M59">
-        <v>0.9999999999980026</v>
+        <v>0.99999999570650944</v>
       </c>
       <c r="N59">
-        <v>0.99999999999977807</v>
+        <v>0.99999999958959285</v>
       </c>
       <c r="O59">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.99999999977288134</v>
+      </c>
+      <c r="P59">
+        <v>0.99999999994758804</v>
+      </c>
+      <c r="Q59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>127</v>
       </c>
@@ -3173,28 +3533,34 @@
         <v>0.99</v>
       </c>
       <c r="I60">
-        <v>0.99874719767901887</v>
+        <v>0.98835274542429286</v>
       </c>
       <c r="J60">
-        <v>0.99983678621661864</v>
+        <v>0.9974811083123426</v>
       </c>
       <c r="K60">
-        <v>0.99996781278294378</v>
+        <v>0.99977823646815989</v>
       </c>
       <c r="L60">
-        <v>0.99999701566755861</v>
+        <v>0.99942927613855426</v>
       </c>
       <c r="M60">
-        <v>0.99999962448699131</v>
+        <v>0.99977978644932097</v>
       </c>
       <c r="N60">
-        <v>0.99999994492474098</v>
+        <v>0.99997518235617089</v>
       </c>
       <c r="O60">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.99998296815103793</v>
+      </c>
+      <c r="P60">
+        <v>0.99999680648412659</v>
+      </c>
+      <c r="Q60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>129</v>
       </c>
@@ -3208,28 +3574,34 @@
         <v>0.99993959587466708</v>
       </c>
       <c r="I61">
-        <v>0.9999892130138226</v>
+        <v>0.999943219916402</v>
       </c>
       <c r="J61">
-        <v>0.9999970845753815</v>
+        <v>0.99998258675551355</v>
       </c>
       <c r="K61">
-        <v>0.99999926191621114</v>
+        <v>0.99999625279491355</v>
       </c>
       <c r="L61">
-        <v>0.99999985238315514</v>
+        <v>0.99999250561791009</v>
       </c>
       <c r="M61">
-        <v>0.99999997047662759</v>
+        <v>0.99999636634617028</v>
       </c>
       <c r="N61">
-        <v>0.99999999205139967</v>
+        <v>0.99999925463295902</v>
       </c>
       <c r="O61">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.99999945078207253</v>
+      </c>
+      <c r="P61">
+        <v>0.99999986095742965</v>
+      </c>
+      <c r="Q61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>131</v>
       </c>
@@ -3243,28 +3615,34 @@
         <v>0.74757499504318092</v>
       </c>
       <c r="I62">
-        <v>0.6012297629357064</v>
+        <v>0.87326033121215874</v>
       </c>
       <c r="J62">
-        <v>0.44362424989006333</v>
+        <v>0.76184899710510157</v>
       </c>
       <c r="K62">
-        <v>0.3264458334623867</v>
+        <v>0.58933466648147093</v>
       </c>
       <c r="L62">
-        <v>0.15229742833167376</v>
+        <v>0.91526006405707561</v>
       </c>
       <c r="M62">
-        <v>8.1730903514066894E-2</v>
+        <v>0.53941933037268064</v>
       </c>
       <c r="N62">
-        <v>4.3347674597570725E-2</v>
+        <v>0.31404515472320932</v>
       </c>
       <c r="O62">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.41567787944981749</v>
+      </c>
+      <c r="P62">
+        <v>0.3216920028230249</v>
+      </c>
+      <c r="Q62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>133</v>
       </c>
@@ -3278,28 +3656,34 @@
         <v>0.99996088009830975</v>
       </c>
       <c r="I63">
-        <v>0.99999383707264844</v>
+        <v>0.99995586494765187</v>
       </c>
       <c r="J63">
-        <v>0.99999883038750914</v>
+        <v>0.99999110917250489</v>
       </c>
       <c r="K63">
-        <v>0.99999980370120911</v>
+        <v>0.9999985617671866</v>
       </c>
       <c r="L63">
-        <v>0.9999999677509076</v>
+        <v>0.99999616472169095</v>
       </c>
       <c r="M63">
-        <v>0.99999999477655532</v>
+        <v>0.99999802049784425</v>
       </c>
       <c r="N63">
-        <v>0.99999999891800073</v>
+        <v>0.99999967256301225</v>
       </c>
       <c r="O63">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.99999977954735109</v>
+      </c>
+      <c r="P63">
+        <v>0.99999995207550285</v>
+      </c>
+      <c r="Q63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>135</v>
       </c>
@@ -3313,28 +3697,34 @@
         <v>0.99998791814778254</v>
       </c>
       <c r="I64">
-        <v>0.99999849962339094</v>
+        <v>0.99998748145979566</v>
       </c>
       <c r="J64">
-        <v>0.9999997707755045</v>
+        <v>0.99999663677930295</v>
       </c>
       <c r="K64">
-        <v>0.99999996074922282</v>
+        <v>0.99999954999028584</v>
       </c>
       <c r="L64">
-        <v>0.99999999364247949</v>
+        <v>0.99999907543502597</v>
       </c>
       <c r="M64">
-        <v>0.99999999928425265</v>
+        <v>0.99999949437831803</v>
       </c>
       <c r="N64">
-        <v>0.99999999984878574</v>
+        <v>0.99999993499146933</v>
       </c>
       <c r="O64">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.99999996427459026</v>
+      </c>
+      <c r="P64">
+        <v>0.99999999208937329</v>
+      </c>
+      <c r="Q64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>137</v>
       </c>
@@ -3360,28 +3750,34 @@
         <v>0.99</v>
       </c>
       <c r="I65">
-        <v>0.99682034976152634</v>
+        <v>0.99</v>
       </c>
       <c r="J65">
-        <v>0.9987350667603655</v>
+        <v>0.99603230834632273</v>
       </c>
       <c r="K65">
-        <v>0.99953177476632094</v>
+        <v>0.99861875182522075</v>
       </c>
       <c r="L65">
-        <v>0.99987057812066182</v>
+        <v>0.99794721739756509</v>
       </c>
       <c r="M65">
-        <v>0.9999550580505886</v>
+        <v>0.99866473195316163</v>
       </c>
       <c r="N65">
-        <v>0.9999887641339259</v>
+        <v>0.99957306807727142</v>
       </c>
       <c r="O65">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.99966452279801477</v>
+      </c>
+      <c r="P65">
+        <v>0.99992128760465437</v>
+      </c>
+      <c r="Q65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>139</v>
       </c>
@@ -3398,28 +3794,34 @@
         <v>0.99</v>
       </c>
       <c r="I66">
-        <v>0.99798387096774188</v>
+        <v>0.9905628197839681</v>
       </c>
       <c r="J66">
-        <v>0.99964445708597027</v>
+        <v>0.99765824286892635</v>
       </c>
       <c r="K66">
-        <v>0.99992787644887504</v>
+        <v>0.99959488294959664</v>
       </c>
       <c r="L66">
-        <v>0.99999018666047845</v>
+        <v>0.99921799995928473</v>
       </c>
       <c r="M66">
-        <v>0.99999830803116896</v>
+        <v>0.99949156081372248</v>
       </c>
       <c r="N66">
-        <v>0.99</v>
+        <v>0.99989674117956728</v>
       </c>
       <c r="O66">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.99993689485344994</v>
+      </c>
+      <c r="P66">
+        <v>0.99998622284473593</v>
+      </c>
+      <c r="Q66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>141</v>
       </c>
@@ -3436,28 +3838,34 @@
         <v>0.99</v>
       </c>
       <c r="I67">
-        <v>0.99145413272800098</v>
+        <v>0.99667676668947325</v>
       </c>
       <c r="J67">
-        <v>0.99284888694317397</v>
+        <v>0.99677140965951794</v>
       </c>
       <c r="K67">
-        <v>0.99489433498052338</v>
+        <v>0.99700466470516158</v>
       </c>
       <c r="L67">
-        <v>0.99457696143045127</v>
+        <v>0.99790137947197177</v>
       </c>
       <c r="M67">
-        <v>0.99552539445672628</v>
+        <v>0.9967160664865834</v>
       </c>
       <c r="N67">
-        <v>0.99617916241438709</v>
+        <v>0.99695679735704446</v>
       </c>
       <c r="O67">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.99872456583239733</v>
+      </c>
+      <c r="P67">
+        <v>0.99881303251772513</v>
+      </c>
+      <c r="Q67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>143</v>
       </c>
@@ -3471,28 +3879,34 @@
         <v>0.99996961921356342</v>
       </c>
       <c r="I68">
-        <v>0.99999466270114989</v>
+        <v>0.99997200864673474</v>
       </c>
       <c r="J68">
-        <v>0.9999988783889916</v>
+        <v>0.99999335442895165</v>
       </c>
       <c r="K68">
-        <v>0.99999972366082235</v>
+        <v>0.99999850099129695</v>
       </c>
       <c r="L68">
-        <v>0.99999995134872521</v>
+        <v>0.99999686571420088</v>
       </c>
       <c r="M68">
-        <v>0.99999999387831606</v>
+        <v>0.9999979627119957</v>
       </c>
       <c r="N68">
-        <v>0.99999999877566326</v>
+        <v>0.99999951041840407</v>
       </c>
       <c r="O68">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.99999970804761451</v>
+      </c>
+      <c r="P68">
+        <v>0.99999994836215067</v>
+      </c>
+      <c r="Q68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>145</v>
       </c>
@@ -3509,28 +3923,34 @@
         <v>0.99</v>
       </c>
       <c r="I69">
-        <v>0.9985304922850845</v>
+        <v>0.98927613941018766</v>
       </c>
       <c r="J69">
-        <v>0.99973913361054734</v>
+        <v>0.99797160243407701</v>
       </c>
       <c r="K69">
-        <v>0.99995321394130976</v>
+        <v>0.999778822228366</v>
       </c>
       <c r="L69">
-        <v>0.99999395257598089</v>
+        <v>0.99945851368775862</v>
       </c>
       <c r="M69">
-        <v>0.99999899904200762</v>
+        <v>0.99971226236256294</v>
       </c>
       <c r="N69">
-        <v>0.99999984651964435</v>
+        <v>0.99996779734985919</v>
       </c>
       <c r="O69">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.99997863454864844</v>
+      </c>
+      <c r="P69">
+        <v>0.99999511638777117</v>
+      </c>
+      <c r="Q69">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>147</v>
       </c>
@@ -3544,28 +3964,34 @@
         <v>0.99998041311255204</v>
       </c>
       <c r="I70">
-        <v>0.99999650228525161</v>
+        <v>0.99997959700889305</v>
       </c>
       <c r="J70">
-        <v>0.99999922777515859</v>
+        <v>0.99999374299421517</v>
       </c>
       <c r="K70">
-        <v>0.99999982839437673</v>
+        <v>0.9999988412893176</v>
       </c>
       <c r="L70">
-        <v>0.99999996567887073</v>
+        <v>0.99999741221650751</v>
       </c>
       <c r="M70">
-        <v>0.99999999207973922</v>
+        <v>0.9999986862005531</v>
       </c>
       <c r="N70">
-        <v>0.9999999983579948</v>
+        <v>0.99999970994008491</v>
       </c>
       <c r="O70">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.99999975828339249</v>
+      </c>
+      <c r="P70">
+        <v>0.9999999568363116</v>
+      </c>
+      <c r="Q70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>149</v>
       </c>
@@ -3579,28 +4005,34 @@
         <v>0.99999703266026885</v>
       </c>
       <c r="I71">
-        <v>0.99999964952588627</v>
+        <v>0.99999632615340461</v>
       </c>
       <c r="J71">
-        <v>0.99999994356771083</v>
+        <v>0.99999923989159312</v>
       </c>
       <c r="K71">
-        <v>0.99999998947872526</v>
+        <v>0.99999993769598872</v>
       </c>
       <c r="L71">
-        <v>0.99999999906666115</v>
+        <v>0.99999981486810352</v>
       </c>
       <c r="M71">
-        <v>0.99999999989462296</v>
+        <v>0.99999992122046122</v>
       </c>
       <c r="N71">
-        <v>0.9999999999866187</v>
+        <v>0.99999999283822327</v>
       </c>
       <c r="O71">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.99999999586208455</v>
+      </c>
+      <c r="P71">
+        <v>0.99999999919345717</v>
+      </c>
+      <c r="Q71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>151</v>
       </c>
@@ -3614,28 +4046,34 @@
         <v>0.99976705619531969</v>
       </c>
       <c r="I72">
-        <v>0.99990292689071181</v>
+        <v>0.99991203907489512</v>
       </c>
       <c r="J72">
-        <v>0.99995946168442296</v>
+        <v>0.99994659330708913</v>
       </c>
       <c r="K72">
-        <v>0.99998335755696555</v>
+        <v>0.99997393173482385</v>
       </c>
       <c r="L72">
-        <v>0.9999906880886118</v>
+        <v>0.99997879770781806</v>
       </c>
       <c r="M72">
-        <v>0.99999565441977045</v>
+        <v>0.99996701904509022</v>
       </c>
       <c r="N72">
-        <v>0.99999777892094177</v>
+        <v>0.99998054943007952</v>
       </c>
       <c r="O72">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.99999425737206526</v>
+      </c>
+      <c r="P72">
+        <v>0.99999734479824109</v>
+      </c>
+      <c r="Q72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>153</v>
       </c>
@@ -3649,28 +4087,34 @@
         <v>0.99999907481074768</v>
       </c>
       <c r="I73">
-        <v>0.99999989255857957</v>
+        <v>0.99999888256384517</v>
       </c>
       <c r="J73">
-        <v>0.99999999093026881</v>
+        <v>0.99999975256749329</v>
       </c>
       <c r="K73">
-        <v>0.99999999829942543</v>
+        <v>0.99999999048336286</v>
       </c>
       <c r="L73">
-        <v>0.99999999990251487</v>
+        <v>0.99999997858756662</v>
       </c>
       <c r="M73">
-        <v>0.99999999998909705</v>
+        <v>0.9999999896182139</v>
       </c>
       <c r="N73">
-        <v>0.99999999999807165</v>
+        <v>0.99999999922838068</v>
       </c>
       <c r="O73">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.99999999961083552</v>
+      </c>
+      <c r="P73">
+        <v>0.999999999914439</v>
+      </c>
+      <c r="Q73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>155</v>
       </c>
@@ -3681,28 +4125,34 @@
         <v>0.9998796670654726</v>
       </c>
       <c r="I74">
-        <v>0.9999832076192513</v>
+        <v>0.9998617094097092</v>
       </c>
       <c r="J74">
-        <v>0.99999658455483731</v>
+        <v>0.99995133783798718</v>
       </c>
       <c r="K74">
-        <v>0.99999925376629195</v>
+        <v>0.99999160963416878</v>
       </c>
       <c r="L74">
-        <v>0.99999983777518608</v>
+        <v>0.9999798234056928</v>
       </c>
       <c r="M74">
-        <v>0.99999997207605296</v>
+        <v>0.99999052925229914</v>
       </c>
       <c r="N74">
-        <v>0.99999999284001351</v>
+        <v>0.99999803757808414</v>
       </c>
       <c r="O74">
+        <v>0.99999879235483269</v>
+      </c>
+      <c r="P74">
+        <v>0.99999977417995023</v>
+      </c>
+      <c r="Q74">
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>157</v>
       </c>
@@ -3713,28 +4163,34 @@
         <v>0.99924448624706907</v>
       </c>
       <c r="I75">
-        <v>0.99979383751567907</v>
+        <v>0.99927530119535557</v>
       </c>
       <c r="J75">
-        <v>0.99993986049312844</v>
+        <v>0.99967537808202056</v>
       </c>
       <c r="K75">
-        <v>0.999981556448857</v>
+        <v>0.99987108077006237</v>
       </c>
       <c r="L75">
-        <v>0.99999229216453367</v>
+        <v>0.99977901595517327</v>
       </c>
       <c r="M75">
-        <v>0.99999794456559088</v>
+        <v>0.9998449132559315</v>
       </c>
       <c r="N75">
-        <v>0.99999917782522241</v>
+        <v>0.99994297722248204</v>
       </c>
       <c r="O75">
+        <v>0.99995723230717837</v>
+      </c>
+      <c r="P75">
+        <v>0.99998761950218051</v>
+      </c>
+      <c r="Q75">
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>159</v>
       </c>
@@ -3748,28 +4204,34 @@
         <v>0.99993893501615194</v>
       </c>
       <c r="I76">
-        <v>0.99998975367663123</v>
+        <v>0.9999511474162851</v>
       </c>
       <c r="J76">
-        <v>0.99999852620083307</v>
+        <v>0.99998706796919079</v>
       </c>
       <c r="K76">
-        <v>0.99999979503429282</v>
+        <v>0.99999743258492013</v>
       </c>
       <c r="L76">
-        <v>0.99999995511699125</v>
+        <v>0.99999563947744519</v>
       </c>
       <c r="M76">
-        <v>0.99999999262197092</v>
+        <v>0.99999691755770259</v>
       </c>
       <c r="N76">
-        <v>0.99999999820819285</v>
+        <v>0.99999934614701558</v>
       </c>
       <c r="O76">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.9999996896967821</v>
+      </c>
+      <c r="P76">
+        <v>0.99999995479024761</v>
+      </c>
+      <c r="Q76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>161</v>
       </c>
@@ -3783,28 +4245,34 @@
         <v>0.99996827557252554</v>
       </c>
       <c r="I77">
-        <v>0.9999948898891019</v>
+        <v>0.99997495423208582</v>
       </c>
       <c r="J77">
-        <v>0.99999891829333565</v>
+        <v>0.99999355427807179</v>
       </c>
       <c r="K77">
-        <v>0.99999980603863281</v>
+        <v>0.99999871084896674</v>
       </c>
       <c r="L77">
-        <v>0.9999999536808607</v>
+        <v>0.99999765804475527</v>
       </c>
       <c r="M77">
-        <v>0.99999999157833797</v>
+        <v>0.99999841223253494</v>
       </c>
       <c r="N77">
-        <v>0.99999999816146812</v>
+        <v>0.9999996184430171</v>
       </c>
       <c r="O77">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.9999997868780458</v>
+      </c>
+      <c r="P77">
+        <v>0.99</v>
+      </c>
+      <c r="Q77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>163</v>
       </c>
@@ -3818,28 +4286,34 @@
         <v>0.97849485883726361</v>
       </c>
       <c r="I78">
-        <v>0.97236103551383524</v>
+        <v>0.9930632696132119</v>
       </c>
       <c r="J78">
-        <v>0.96926992585327754</v>
+        <v>0.99035404521918069</v>
       </c>
       <c r="K78">
-        <v>0.96556095588234703</v>
+        <v>0.98507516162764264</v>
       </c>
       <c r="L78">
-        <v>0.94540547067858449</v>
+        <v>0.9956242948047298</v>
       </c>
       <c r="M78">
-        <v>0.93466284372544628</v>
+        <v>0.98205425302473759</v>
       </c>
       <c r="N78">
-        <v>0.91886390825991338</v>
+        <v>0.96995812511479995</v>
       </c>
       <c r="O78">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.98564929323774286</v>
+      </c>
+      <c r="P78">
+        <v>0.98370821836280764</v>
+      </c>
+      <c r="Q78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>165</v>
       </c>
@@ -3850,28 +4324,34 @@
         <v>0.99999343419507891</v>
       </c>
       <c r="I79">
-        <v>0.99999900991278501</v>
+        <v>0.99999379396297883</v>
       </c>
       <c r="J79">
-        <v>0.99999986089671922</v>
+        <v>0.99999862087400504</v>
       </c>
       <c r="K79">
-        <v>0.99999997333853485</v>
+        <v>0.99999980131212218</v>
       </c>
       <c r="L79">
-        <v>0.99999999609832213</v>
+        <v>0.99999961504230839</v>
       </c>
       <c r="M79">
-        <v>0.99999999950058516</v>
+        <v>0.99999974627785171</v>
       </c>
       <c r="N79">
-        <v>0.99999999989595523</v>
+        <v>0.99999995469246405</v>
       </c>
       <c r="O79">
+        <v>0.99999997541825125</v>
+      </c>
+      <c r="P79">
+        <v>0.99999999556722552</v>
+      </c>
+      <c r="Q79">
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>167</v>
       </c>
@@ -3885,28 +4365,34 @@
         <v>0.99999785978255051</v>
       </c>
       <c r="I80">
-        <v>0.99</v>
+        <v>0.99999788466874717</v>
       </c>
       <c r="J80">
-        <v>0.99838924294418385</v>
+        <v>0.99999957101601544</v>
       </c>
       <c r="K80">
-        <v>0.99971277258985947</v>
+        <v>0.99999996282137338</v>
       </c>
       <c r="L80">
-        <v>0.999965292622082</v>
+        <v>0.99999992013480554</v>
       </c>
       <c r="M80">
-        <v>0.99999688513690843</v>
+        <v>0.99999995632372018</v>
       </c>
       <c r="N80">
-        <v>0.99999937702582931</v>
+        <v>0.99999999548176388</v>
       </c>
       <c r="O80">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.99999999743559576</v>
+      </c>
+      <c r="P80">
+        <v>0.99999999958694152</v>
+      </c>
+      <c r="Q80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>169</v>
       </c>
@@ -3920,28 +4406,34 @@
         <v>0.99177033431837991</v>
       </c>
       <c r="I81">
-        <v>0.99274717944147695</v>
+        <v>0.99785329656283528</v>
       </c>
       <c r="J81">
-        <v>0.99371894553553186</v>
+        <v>0.9979271673793958</v>
       </c>
       <c r="K81">
-        <v>0.9944739982697397</v>
+        <v>0.9979271673793958</v>
       </c>
       <c r="L81">
-        <v>0.99346270520670155</v>
+        <v>0.9992237870696915</v>
       </c>
       <c r="M81">
-        <v>0.99411989277063773</v>
+        <v>0.99782368662956433</v>
       </c>
       <c r="N81">
-        <v>0.99444840194128292</v>
+        <v>0.99768269505886897</v>
       </c>
       <c r="O81">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.99920839270521788</v>
+      </c>
+      <c r="P81">
+        <v>0.99934304585331779</v>
+      </c>
+      <c r="Q81">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>171</v>
       </c>
@@ -3955,28 +4447,34 @@
         <v>0.99996313099936573</v>
       </c>
       <c r="I82">
-        <v>0.99999349350821576</v>
+        <v>0.99996738497607551</v>
       </c>
       <c r="J82">
-        <v>0.99999896847736225</v>
+        <v>0.99998776911670917</v>
       </c>
       <c r="K82">
-        <v>0.99999983207756504</v>
+        <v>0.99999758399934091</v>
       </c>
       <c r="L82">
-        <v>0.99999995909581196</v>
+        <v>0.99999640697760783</v>
       </c>
       <c r="M82">
-        <v>0.99999999192016009</v>
+        <v>0.99999735250731303</v>
       </c>
       <c r="N82">
-        <v>0.99999999810472895</v>
+        <v>0.99999929400057952</v>
       </c>
       <c r="O82">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.999999619846342</v>
+      </c>
+      <c r="P82">
+        <v>0.9999999275897572</v>
+      </c>
+      <c r="Q82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>173</v>
       </c>
@@ -3990,28 +4488,34 @@
         <v>0.99848377865164628</v>
       </c>
       <c r="I83">
-        <v>0.9996394806265485</v>
+        <v>0.9986876175055307</v>
       </c>
       <c r="J83">
-        <v>0.99985468479640238</v>
+        <v>0.99944799898843195</v>
       </c>
       <c r="K83">
-        <v>0.99994268755182192</v>
+        <v>0.99983582791001613</v>
       </c>
       <c r="L83">
-        <v>0.99998089512064237</v>
+        <v>0.99974944319656889</v>
       </c>
       <c r="M83">
-        <v>0.99999290381673633</v>
+        <v>0.99986078627322872</v>
       </c>
       <c r="N83">
-        <v>0.99999676496278589</v>
+        <v>0.99995745835961136</v>
       </c>
       <c r="O83">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.99996733377495572</v>
+      </c>
+      <c r="P83">
+        <v>0.99999274065444033</v>
+      </c>
+      <c r="Q83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>175</v>
       </c>
@@ -4025,28 +4529,34 @@
         <v>0.99999612709972119</v>
       </c>
       <c r="I84">
-        <v>0.99999965243080091</v>
+        <v>0.9999959854088164</v>
       </c>
       <c r="J84">
-        <v>0.99999995685346554</v>
+        <v>0.99999905538740974</v>
       </c>
       <c r="K84">
-        <v>0.99999999209993007</v>
+        <v>0.99999990879594802</v>
       </c>
       <c r="L84">
-        <v>0.99999999914012838</v>
+        <v>0.99999979434382802</v>
       </c>
       <c r="M84">
-        <v>0.99</v>
+        <v>0.99999987660628664</v>
       </c>
       <c r="N84">
-        <v>0.99826147426981915</v>
+        <v>0.99999998501647613</v>
       </c>
       <c r="O84">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.99999999263967243</v>
+      </c>
+      <c r="P84">
+        <v>0.99999999866175859</v>
+      </c>
+      <c r="Q84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>177</v>
       </c>
@@ -4060,28 +4570,34 @@
         <v>0.99999784383749635</v>
       </c>
       <c r="I85">
-        <v>0.99999970210857425</v>
+        <v>0.99999726886239904</v>
       </c>
       <c r="J85">
-        <v>0.99999995208738102</v>
+        <v>0.99999951027767742</v>
       </c>
       <c r="K85">
-        <v>0.99999999217753122</v>
+        <v>0.99999994633177691</v>
       </c>
       <c r="L85">
-        <v>0.99999999898893266</v>
+        <v>0.99999985211424358</v>
       </c>
       <c r="M85">
-        <v>0.99999999985750054</v>
+        <v>0.99999992605711641</v>
       </c>
       <c r="N85">
-        <v>0.99999999997704703</v>
+        <v>0.99999999003606477</v>
       </c>
       <c r="O85">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.99999999354716584</v>
+      </c>
+      <c r="P85">
+        <v>0.99999999900392489</v>
+      </c>
+      <c r="Q85">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>179</v>
       </c>
@@ -4092,28 +4608,34 @@
         <v>0.9999983318744694</v>
       </c>
       <c r="I86">
-        <v>0.99999985172194972</v>
+        <v>0.99999791484395628</v>
       </c>
       <c r="J86">
-        <v>0.99999998086734587</v>
+        <v>0.99999958641463893</v>
       </c>
       <c r="K86">
-        <v>0.99999999620509328</v>
+        <v>0.99999997435128551</v>
       </c>
       <c r="L86">
-        <v>0.99999999977000575</v>
+        <v>0.9999999459146689</v>
       </c>
       <c r="M86">
-        <v>0.99999999997700051</v>
+        <v>0.99999997350922487</v>
       </c>
       <c r="N86">
-        <v>0.99999999999637801</v>
+        <v>0.99999999715388366</v>
       </c>
       <c r="O86">
+        <v>0.99999999853292976</v>
+      </c>
+      <c r="P86">
+        <v>0.99999999966713526</v>
+      </c>
+      <c r="Q86">
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>181</v>
       </c>
@@ -4127,28 +4649,34 @@
         <v>0.72493945755884703</v>
       </c>
       <c r="I87">
-        <v>0.61114703925608327</v>
+        <v>0.86446307238879927</v>
       </c>
       <c r="J87">
-        <v>0.54362021195601851</v>
+        <v>0.79485177635374882</v>
       </c>
       <c r="K87">
-        <v>0.4970849271006253</v>
+        <v>0.68155030680200002</v>
       </c>
       <c r="L87">
-        <v>0.33870074209531498</v>
+        <v>0.89883793556760283</v>
       </c>
       <c r="M87">
-        <v>0.2453023491400613</v>
+        <v>0.69225083964048273</v>
       </c>
       <c r="N87">
-        <v>0.16571547854268959</v>
+        <v>0.52700529881676128</v>
       </c>
       <c r="O87">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.63461288587548714</v>
+      </c>
+      <c r="P87">
+        <v>0.54729936233300391</v>
+      </c>
+      <c r="Q87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>183</v>
       </c>
@@ -4162,28 +4690,34 @@
         <v>0.99108962728540162</v>
       </c>
       <c r="I88">
-        <v>0.99015105123112279</v>
+        <v>0.99736972873763419</v>
       </c>
       <c r="J88">
-        <v>0.99268580610280011</v>
+        <v>0.99747467389642175</v>
       </c>
       <c r="K88">
-        <v>0.99437419169883479</v>
+        <v>0.99725568295658595</v>
       </c>
       <c r="L88">
-        <v>0.99362886296476216</v>
+        <v>0.99856061958859499</v>
       </c>
       <c r="M88">
-        <v>0.99460374862295264</v>
+        <v>0.99716880843734279</v>
       </c>
       <c r="N88">
-        <v>0.99491956250879021</v>
+        <v>0.99649707650514896</v>
       </c>
       <c r="O88">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.9989966542562001</v>
+      </c>
+      <c r="P88">
+        <v>0.99901670143930754</v>
+      </c>
+      <c r="Q88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>185</v>
       </c>
@@ -4197,28 +4731,34 @@
         <v>0.99999989897666763</v>
       </c>
       <c r="I89">
-        <v>0.99999999679290985</v>
+        <v>0.99999983583709529</v>
       </c>
       <c r="J89">
-        <v>0.99999999972352671</v>
+        <v>0.99999998631975595</v>
       </c>
       <c r="K89">
-        <v>0.99999999994880118</v>
+        <v>0.9999999997466622</v>
       </c>
       <c r="L89">
-        <v>0.99999999999948275</v>
+        <v>0.99999999888109148</v>
       </c>
       <c r="M89">
-        <v>0.9999999999999919</v>
+        <v>0.99999999973672749</v>
       </c>
       <c r="N89">
-        <v>0.99999999999999889</v>
+        <v>0.99999999997649347</v>
       </c>
       <c r="O89">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.99999999997985145</v>
+      </c>
+      <c r="P89">
+        <v>0.99999999999670297</v>
+      </c>
+      <c r="Q89">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>187</v>
       </c>
@@ -4232,28 +4772,34 @@
         <v>0.99999865871045135</v>
       </c>
       <c r="I90">
-        <v>0.9999998624316756</v>
+        <v>0.99999835868565001</v>
       </c>
       <c r="J90">
-        <v>0.99999998724531936</v>
+        <v>0.99999969010107381</v>
       </c>
       <c r="K90">
-        <v>0.99999999829937591</v>
+        <v>0.9999999772740723</v>
       </c>
       <c r="L90">
-        <v>0.99999999982993759</v>
+        <v>0.99999994149282645</v>
       </c>
       <c r="M90">
-        <v>0.99999999998463951</v>
+        <v>0.99999996602809205</v>
       </c>
       <c r="N90">
-        <v>0.9999999999976289</v>
+        <v>0.99999999646125948</v>
       </c>
       <c r="O90">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.99999999790296867</v>
+      </c>
+      <c r="P90">
+        <v>0.99999999955382313</v>
+      </c>
+      <c r="Q90">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>189</v>
       </c>
@@ -4267,28 +4813,34 @@
         <v>0.99999872673798607</v>
       </c>
       <c r="I91">
-        <v>0.99999985944494307</v>
+        <v>0.99999842115558513</v>
       </c>
       <c r="J91">
-        <v>0.9999999826712922</v>
+        <v>0.99999960236464069</v>
       </c>
       <c r="K91">
-        <v>0.99999999641048187</v>
+        <v>0.9999999818075257</v>
       </c>
       <c r="L91">
-        <v>0.99999999976691445</v>
+        <v>0.99999995355113069</v>
       </c>
       <c r="M91">
-        <v>0.99999999997358369</v>
+        <v>0.99999997989526501</v>
       </c>
       <c r="N91">
-        <v>0.99999999999568712</v>
+        <v>0.99999999863233102</v>
       </c>
       <c r="O91">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.99999999918195503</v>
+      </c>
+      <c r="P91">
+        <v>0.99999999981755838</v>
+      </c>
+      <c r="Q91">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>191</v>
       </c>
@@ -4302,28 +4854,34 @@
         <v>0.99999731697299354</v>
       </c>
       <c r="I92">
-        <v>0.9999997224448145</v>
+        <v>0.99999691268250102</v>
       </c>
       <c r="J92">
-        <v>0.99999995857384316</v>
+        <v>0.99999921591755936</v>
       </c>
       <c r="K92">
-        <v>0.99999999258038952</v>
+        <v>0.99999996710141137</v>
       </c>
       <c r="L92">
-        <v>0.99999999931103623</v>
+        <v>0.99999991885015194</v>
       </c>
       <c r="M92">
-        <v>0.99999999991634003</v>
+        <v>0.99999996006912073</v>
       </c>
       <c r="N92">
-        <v>0.99999999998301647</v>
+        <v>0.99</v>
       </c>
       <c r="O92">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.99397590361445776</v>
+      </c>
+      <c r="P92">
+        <v>0.99854569337586785</v>
+      </c>
+      <c r="Q92">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>193</v>
       </c>
@@ -4337,28 +4895,34 @@
         <v>0.98930337485637709</v>
       </c>
       <c r="I93">
-        <v>0.98595938234522573</v>
+        <v>0.99775832883659865</v>
       </c>
       <c r="J93">
-        <v>0.98533053464974429</v>
+        <v>0.99766109283213567</v>
       </c>
       <c r="K93">
-        <v>0.98563175737709752</v>
+        <v>0.99682415159762783</v>
       </c>
       <c r="L93">
-        <v>0.97933668106834315</v>
+        <v>0.99867834758712615</v>
       </c>
       <c r="M93">
-        <v>0.977500462539861</v>
+        <v>0.99480319461974642</v>
       </c>
       <c r="N93">
-        <v>0.97057637101719874</v>
+        <v>0.99379547526896594</v>
       </c>
       <c r="O93">
+        <v>0.99789404624894418</v>
+      </c>
+      <c r="P93">
+        <v>0.99745438728904257</v>
+      </c>
+      <c r="Q93">
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>195</v>
       </c>
@@ -4369,28 +4933,34 @@
         <v>0.99999640146876112</v>
       </c>
       <c r="I94">
-        <v>0.9999995411254482</v>
+        <v>0.99999578593311678</v>
       </c>
       <c r="J94">
-        <v>0.99999992407108829</v>
+        <v>0.9999989936524416</v>
       </c>
       <c r="K94">
-        <v>0.99999998325097439</v>
+        <v>0.99999993154091826</v>
       </c>
       <c r="L94">
-        <v>0.99999999853867561</v>
+        <v>0.99999981329343546</v>
       </c>
       <c r="M94">
-        <v>0.99999999980851606</v>
+        <v>0.99999991513337116</v>
       </c>
       <c r="N94">
-        <v>0.9999999999649396</v>
+        <v>0.99999999483919111</v>
       </c>
       <c r="O94">
+        <v>0.99999999682411755</v>
+      </c>
+      <c r="P94">
+        <v>0.99999999918812021</v>
+      </c>
+      <c r="Q94">
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>197</v>
       </c>
@@ -4404,28 +4974,34 @@
         <v>0.85614581649702148</v>
       </c>
       <c r="I95">
-        <v>0.73222405872207852</v>
+        <v>0.92316710940399627</v>
       </c>
       <c r="J95">
-        <v>0.57992138960020911</v>
+        <v>0.84898408442318041</v>
       </c>
       <c r="K95">
-        <v>0.43977405179125073</v>
+        <v>0.70472043720048683</v>
       </c>
       <c r="L95">
-        <v>0.22433018356421414</v>
+        <v>0.96714308499008461</v>
       </c>
       <c r="M95">
-        <v>0.1242480072886497</v>
+        <v>0.71532221481072333</v>
       </c>
       <c r="N95">
-        <v>5.9564731369920132E-2</v>
+        <v>0.50715323551105906</v>
       </c>
       <c r="O95">
+        <v>0.58105551427163538</v>
+      </c>
+      <c r="P95">
+        <v>0.45829997822577345</v>
+      </c>
+      <c r="Q95">
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>199</v>
       </c>
@@ -4439,28 +5015,34 @@
         <v>0.64413457594871459</v>
       </c>
       <c r="I96">
-        <v>0.41083408003454486</v>
+        <v>0.8208814650946451</v>
       </c>
       <c r="J96">
-        <v>0.25320819633071667</v>
+        <v>0.65553666957700352</v>
       </c>
       <c r="K96">
-        <v>0.15284242244804394</v>
+        <v>0.40007916448484104</v>
       </c>
       <c r="L96">
-        <v>4.8653833526706269E-2</v>
+        <v>0.86131108193996231</v>
       </c>
       <c r="M96">
-        <v>2.0550199858803277E-2</v>
+        <v>0.43984515026986587</v>
       </c>
       <c r="N96">
-        <v>9.7560047923658886E-3</v>
+        <v>0.22591747186773761</v>
       </c>
       <c r="O96">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.26315340400041853</v>
+      </c>
+      <c r="P96">
+        <v>0.16555971440514397</v>
+      </c>
+      <c r="Q96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>201</v>
       </c>
@@ -4474,28 +5056,34 @@
         <v>0.79939407810678953</v>
       </c>
       <c r="I97">
-        <v>0.64974203699408273</v>
+        <v>0.90139840869457</v>
       </c>
       <c r="J97">
-        <v>0.45790792488057158</v>
+        <v>0.80683300919739054</v>
       </c>
       <c r="K97">
-        <v>0.31939480903210266</v>
+        <v>0.62967323475381032</v>
       </c>
       <c r="L97">
-        <v>0.14680831125156674</v>
+        <v>0.99</v>
       </c>
       <c r="M97">
-        <v>7.0898875679580517E-2</v>
+        <v>0.9339622641509433</v>
       </c>
       <c r="N97">
-        <v>3.8014969589016283E-2</v>
+        <v>0.85149082568807322</v>
       </c>
       <c r="O97">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="98" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.88641596316193383</v>
+      </c>
+      <c r="P97">
+        <v>0.81117145800168533</v>
+      </c>
+      <c r="Q97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>203</v>
       </c>
@@ -4515,28 +5103,34 @@
         <v>0.99</v>
       </c>
       <c r="I98">
-        <v>0.98890122086570476</v>
+        <v>0.99836127568385236</v>
       </c>
       <c r="J98">
-        <v>0.98960228749675072</v>
+        <v>0.99852490638829017</v>
       </c>
       <c r="K98">
-        <v>0.99023266430622714</v>
+        <v>0.99816578736966177</v>
       </c>
       <c r="L98">
-        <v>0.98677281868493971</v>
+        <v>0.9991116367545666</v>
       </c>
       <c r="M98">
-        <v>0.98677281868493971</v>
+        <v>0.99767991786498933</v>
       </c>
       <c r="N98">
-        <v>0.98592232042658012</v>
+        <v>0.9974646434557255</v>
       </c>
       <c r="O98">
+        <v>0.99914153728184651</v>
+      </c>
+      <c r="P98">
+        <v>0.99912328813091678</v>
+      </c>
+      <c r="Q98">
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>205</v>
       </c>
@@ -4562,28 +5156,34 @@
         <v>0.5</v>
       </c>
       <c r="I99">
-        <v>0.35353535353535354</v>
+        <v>0.72164948453608246</v>
       </c>
       <c r="J99">
-        <v>0.25341914722445696</v>
+        <v>0.6112815671465659</v>
       </c>
       <c r="K99">
-        <v>0.18707684998218313</v>
+        <v>0.40499517413552311</v>
       </c>
       <c r="L99">
-        <v>9.0584919767642477E-2</v>
+        <v>0.82652774087867209</v>
       </c>
       <c r="M99">
-        <v>5.6394342662767778E-2</v>
+        <v>0.01</v>
       </c>
       <c r="N99">
-        <v>3.7394414428125702E-2</v>
+        <v>4.9457562220804078E-3</v>
       </c>
       <c r="O99">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="100" spans="1:15" x14ac:dyDescent="0.25">
+        <v>9.006759609404438E-3</v>
+      </c>
+      <c r="P99">
+        <v>6.1240403695876884E-3</v>
+      </c>
+      <c r="Q99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>207</v>
       </c>
@@ -4609,28 +5209,34 @@
         <v>0.33333333333333337</v>
       </c>
       <c r="I100">
-        <v>0.20524017467248912</v>
+        <v>0.55428571428571438</v>
       </c>
       <c r="J100">
-        <v>0.12120713305898492</v>
+        <v>0.37821679230569277</v>
       </c>
       <c r="K100">
-        <v>7.6976687458619381E-2</v>
+        <v>0.20860215053763442</v>
       </c>
       <c r="L100">
-        <v>3.1324376829917247E-2</v>
+        <v>0.73145220141084888</v>
       </c>
       <c r="M100">
-        <v>1.809142395554366E-2</v>
+        <v>0.19053524390575077</v>
       </c>
       <c r="N100">
-        <v>8.2706513559150704E-3</v>
+        <v>8.8609008438140832E-2</v>
       </c>
       <c r="O100">
+        <v>0.146112240668717</v>
+      </c>
+      <c r="P100">
+        <v>9.7444293844978505E-2</v>
+      </c>
+      <c r="Q100">
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>209</v>
       </c>
@@ -4644,28 +5250,34 @@
         <v>0.99364481100148005</v>
       </c>
       <c r="I101">
-        <v>0.991394632336973</v>
+        <v>0.99901114707578886</v>
       </c>
       <c r="J101">
-        <v>0.99023263471511147</v>
+        <v>0.99901114707578886</v>
       </c>
       <c r="K101">
-        <v>0.98920477042422983</v>
+        <v>0.99853010633487405</v>
       </c>
       <c r="L101">
-        <v>0.98289577362537883</v>
+        <v>0.99936324652589903</v>
       </c>
       <c r="M101">
-        <v>0.97900157257458209</v>
+        <v>0.99792661485532674</v>
       </c>
       <c r="N101">
-        <v>0.97588322276583173</v>
+        <v>0.99694748301786484</v>
       </c>
       <c r="O101">
+        <v>0.99873312076475007</v>
+      </c>
+      <c r="P101">
+        <v>0.99848013001604474</v>
+      </c>
+      <c r="Q101">
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>211</v>
       </c>
@@ -4673,28 +5285,58 @@
         <v>83.516483516483518</v>
       </c>
       <c r="I102">
-        <v>85.714285714285722</v>
+        <v>84.615384615384613</v>
       </c>
       <c r="J102">
-        <v>85.714285714285722</v>
+        <v>83.516483516483518</v>
       </c>
       <c r="K102">
         <v>85.714285714285722</v>
       </c>
       <c r="L102">
-        <v>86.813186813186817</v>
+        <v>84.615384615384613</v>
       </c>
       <c r="M102">
         <v>85.714285714285722</v>
       </c>
       <c r="N102">
+        <v>89.010989010989007</v>
+      </c>
+      <c r="O102">
+        <v>86.813186813186817</v>
+      </c>
+      <c r="P102">
         <v>87.912087912087912</v>
       </c>
-      <c r="O102">
+      <c r="Q102">
         <v>87.912087912087912</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="H2:Q101">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H102:Q102">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>